<commit_message>
intellecx data fill 2
</commit_message>
<xml_diff>
--- a/QUIZ REGISTRATION.xlsx
+++ b/QUIZ REGISTRATION.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="220">
   <si>
     <t>INX1002</t>
   </si>
@@ -670,13 +670,22 @@
   </si>
   <si>
     <t>anunay.jain.civ15@iitbhu.ac.in</t>
+  </si>
+  <si>
+    <t>INX1097</t>
+  </si>
+  <si>
+    <t>varunsethi1911@gmail.com</t>
+  </si>
+  <si>
+    <t>opopopopo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -685,6 +694,23 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -704,14 +730,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -992,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1020,6 +1051,9 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1028,6 +1062,9 @@
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1047,6 +1084,9 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1088,6 +1128,9 @@
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1107,6 +1150,9 @@
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1126,6 +1172,9 @@
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1134,6 +1183,9 @@
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1142,6 +1194,9 @@
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1150,6 +1205,9 @@
       <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C16" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1158,6 +1216,9 @@
       <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C17" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1166,6 +1227,9 @@
       <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="C18" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1174,6 +1238,9 @@
       <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1182,6 +1249,9 @@
       <c r="B20" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="C20" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1190,6 +1260,9 @@
       <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1198,6 +1271,9 @@
       <c r="B22" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="C22" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1206,6 +1282,9 @@
       <c r="B23" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C23" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1214,6 +1293,9 @@
       <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C24" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1222,6 +1304,9 @@
       <c r="B25" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C25" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1241,6 +1326,9 @@
       <c r="B27" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="C27" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1249,6 +1337,9 @@
       <c r="B28" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1257,6 +1348,9 @@
       <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1265,6 +1359,9 @@
       <c r="B30" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="C30" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1273,6 +1370,9 @@
       <c r="B31" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C31" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1281,6 +1381,9 @@
       <c r="B32" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="C32" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1289,6 +1392,9 @@
       <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C33" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1319,6 +1425,9 @@
       <c r="B36" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="C36" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1327,6 +1436,9 @@
       <c r="B37" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="C37" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1335,6 +1447,9 @@
       <c r="B38" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="C38" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1365,6 +1480,9 @@
       <c r="B41" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="C41" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="42" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -1384,6 +1502,9 @@
       <c r="B43" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="C43" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -1403,6 +1524,9 @@
       <c r="B45" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="C45" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1422,6 +1546,9 @@
       <c r="B47" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="C47" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -1430,6 +1557,9 @@
       <c r="B48" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="C48" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -1438,6 +1568,9 @@
       <c r="B49" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="C49" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="50" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -1446,6 +1579,9 @@
       <c r="B50" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="C50" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="51" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -1454,6 +1590,9 @@
       <c r="B51" s="1" t="s">
         <v>116</v>
       </c>
+      <c r="C51" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="52" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
@@ -1462,6 +1601,9 @@
       <c r="B52" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="C52" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="53" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -1470,6 +1612,9 @@
       <c r="B53" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="C53" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="54" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
@@ -1478,6 +1623,9 @@
       <c r="B54" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="C54" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="55" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -1486,6 +1634,9 @@
       <c r="B55" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="C55" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="56" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -1505,6 +1656,9 @@
       <c r="B57" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="C57" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="58" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -1535,6 +1689,9 @@
       <c r="B60" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="C60" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="61" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -1554,6 +1711,9 @@
       <c r="B62" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="C62" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="63" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -1562,6 +1722,9 @@
       <c r="B63" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="C63" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -1570,6 +1733,9 @@
       <c r="B64" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="C64" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="65" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -1578,6 +1744,9 @@
       <c r="B65" s="1" t="s">
         <v>148</v>
       </c>
+      <c r="C65" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="66" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -1619,6 +1788,9 @@
       <c r="B69" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="C69" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="70" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -1627,6 +1799,9 @@
       <c r="B70" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="C70" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="71" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
@@ -1635,6 +1810,9 @@
       <c r="B71" s="1" t="s">
         <v>163</v>
       </c>
+      <c r="C71" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="72" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
@@ -1643,6 +1821,9 @@
       <c r="B72" s="1" t="s">
         <v>165</v>
       </c>
+      <c r="C72" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="73" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -1651,6 +1832,9 @@
       <c r="B73" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="C73" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="74" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
@@ -1659,6 +1843,9 @@
       <c r="B74" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="C74" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
@@ -1678,6 +1865,9 @@
       <c r="B76" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="C76" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="77" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -1697,6 +1887,9 @@
       <c r="B78" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="C78" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="79" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
@@ -1705,6 +1898,9 @@
       <c r="B79" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="C79" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="80" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -1721,8 +1917,11 @@
       <c r="A81" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="2" t="s">
         <v>186</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -1732,6 +1931,9 @@
       <c r="B82" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="C82" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="83" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
@@ -1740,6 +1942,9 @@
       <c r="B83" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="C83" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="84" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
@@ -1748,6 +1953,9 @@
       <c r="B84" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="C84" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="85" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
@@ -1756,6 +1964,9 @@
       <c r="B85" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="C85" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
@@ -1775,6 +1986,9 @@
       <c r="B87" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="C87" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="88" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
@@ -1783,6 +1997,9 @@
       <c r="B88" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="C88" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="89" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
@@ -1791,6 +2008,9 @@
       <c r="B89" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="C89" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="90" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
@@ -1799,6 +2019,9 @@
       <c r="B90" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="C90" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="91" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
@@ -1807,6 +2030,9 @@
       <c r="B91" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="C91" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="92" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
@@ -1842,7 +2068,15 @@
       </c>
     </row>
     <row r="95" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
+      <c r="A95" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="96" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
@@ -1911,6 +2145,11 @@
       <c r="A110" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B81" r:id="rId1"/>
+    <hyperlink ref="B95" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>